<commit_message>
Indicated the common failures WS CoE sees regularly, or could see regularly.
</commit_message>
<xml_diff>
--- a/priorities/axe_rules.xlsx
+++ b/priorities/axe_rules.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="427">
   <si>
     <t>url</t>
   </si>
@@ -1680,11 +1680,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F170"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B142" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B103" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B170" sqref="B170"/>
+      <selection pane="bottomRight" activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4510,6 +4510,9 @@
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>219</v>
+      </c>
       <c r="B156" t="s">
         <v>229</v>
       </c>
@@ -4521,6 +4524,9 @@
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>219</v>
+      </c>
       <c r="B157" t="s">
         <v>393</v>
       </c>
@@ -4598,6 +4604,9 @@
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>219</v>
+      </c>
       <c r="B164" t="s">
         <v>241</v>
       </c>
@@ -4609,6 +4618,9 @@
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>219</v>
+      </c>
       <c r="B165" t="s">
         <v>242</v>
       </c>
@@ -4667,6 +4679,9 @@
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>219</v>
+      </c>
       <c r="B170" t="s">
         <v>392</v>
       </c>

</xml_diff>

<commit_message>
Add definitions of impact add drop down impact list
</commit_message>
<xml_diff>
--- a/priorities/axe_rules.xlsx
+++ b/priorities/axe_rules.xlsx
@@ -1,38 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nordlund\Documents\CLF2.0\documentations\ITAO Git Repos Fork\example\priorities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shawnthompson/git/github/bati-itao/example/priorities/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37324795-ED3E-6349-923F-F1790A493EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67995" yWindow="-5115" windowWidth="34395" windowHeight="28335"/>
+    <workbookView xWindow="33560" yWindow="-5120" windowWidth="68800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Definitions" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="impact">Definitions!$A$2:$A$5</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="432">
   <si>
     <t>url</t>
   </si>
@@ -1313,13 +1310,28 @@
   </si>
   <si>
     <t>A webpage or web app that includes single-key shortcuts not including a control that allows users to turn the shortcuts off or a control that allows users to change the shortcuts to key combinations that include keys that are not upper or lower-case letters, punctuation, number, or symbol characters.</t>
+  </si>
+  <si>
+    <t>This issue results in blocked content for individuals with disabilities. Until a solution is implemented content will be completely inaccessible, making your organization highly vulnerable to legal action. Remediation should be a top priority.</t>
+  </si>
+  <si>
+    <t>This issue results in serious barriers for individuals with disabilities. Until a solution is implemented some content will be inaccessible, making your organization vulnerable to legal action. Users relying on Assistive Technology will experience significant frustration when attempting to access content. Remediation should be a priority.</t>
+  </si>
+  <si>
+    <t>This issue results in some barriers for individuals with disabilities but would not prevent them from accessing fundamental elements or content. This might make your organization vulnerable to legal action. This issue must be resolved before a page can be considered fully compliant.</t>
+  </si>
+  <si>
+    <t>This is considered an Accessibility issue that yields less impact for users than a moderate issue. For a page to be considered fully compliant this issue must be resolved but can be dealt with last.</t>
+  </si>
+  <si>
+    <t>Definitions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1335,16 +1347,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1352,17 +1378,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1677,24 +1727,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F170"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B103" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="202" zoomScaleNormal="202" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A106" sqref="A106"/>
+      <selection pane="bottomRight" activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="38" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="121" customWidth="1"/>
-    <col min="4" max="4" width="20.75" customWidth="1"/>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>218</v>
       </c>
@@ -1714,7 +1765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>219</v>
       </c>
@@ -1734,7 +1785,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>219</v>
       </c>
@@ -1754,7 +1805,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>219</v>
       </c>
@@ -1774,7 +1825,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>219</v>
       </c>
@@ -1794,7 +1845,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>219</v>
       </c>
@@ -1814,7 +1865,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -1834,7 +1885,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>219</v>
       </c>
@@ -1854,7 +1905,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>219</v>
       </c>
@@ -1874,7 +1925,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>219</v>
       </c>
@@ -1894,7 +1945,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>219</v>
       </c>
@@ -1914,7 +1965,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>219</v>
       </c>
@@ -1934,7 +1985,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>219</v>
       </c>
@@ -1954,7 +2005,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>219</v>
       </c>
@@ -1974,7 +2025,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>219</v>
       </c>
@@ -1994,7 +2045,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>219</v>
       </c>
@@ -2014,7 +2065,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>219</v>
       </c>
@@ -2034,7 +2085,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>219</v>
       </c>
@@ -2054,7 +2105,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>219</v>
       </c>
@@ -2074,7 +2125,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>219</v>
       </c>
@@ -2094,7 +2145,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>219</v>
       </c>
@@ -2114,7 +2165,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>219</v>
       </c>
@@ -2134,7 +2185,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>219</v>
       </c>
@@ -2154,7 +2205,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>219</v>
       </c>
@@ -2174,7 +2225,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>219</v>
       </c>
@@ -2194,7 +2245,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>219</v>
       </c>
@@ -2214,7 +2265,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>219</v>
       </c>
@@ -2234,7 +2285,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>219</v>
       </c>
@@ -2254,7 +2305,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>219</v>
       </c>
@@ -2274,7 +2325,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>219</v>
       </c>
@@ -2294,7 +2345,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>219</v>
       </c>
@@ -2314,7 +2365,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>219</v>
       </c>
@@ -2334,7 +2385,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>219</v>
       </c>
@@ -2354,7 +2405,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>219</v>
       </c>
@@ -2374,7 +2425,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>219</v>
       </c>
@@ -2394,7 +2445,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>219</v>
       </c>
@@ -2414,7 +2465,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>219</v>
       </c>
@@ -2434,7 +2485,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>219</v>
       </c>
@@ -2454,7 +2505,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>219</v>
       </c>
@@ -2474,7 +2525,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>219</v>
       </c>
@@ -2494,7 +2545,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>219</v>
       </c>
@@ -2514,7 +2565,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>219</v>
       </c>
@@ -2534,7 +2585,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>219</v>
       </c>
@@ -2554,7 +2605,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>219</v>
       </c>
@@ -2574,7 +2625,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>219</v>
       </c>
@@ -2594,7 +2645,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>219</v>
       </c>
@@ -2614,7 +2665,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>219</v>
       </c>
@@ -2634,7 +2685,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>219</v>
       </c>
@@ -2654,7 +2705,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>219</v>
       </c>
@@ -2674,7 +2725,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>219</v>
       </c>
@@ -2694,7 +2745,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>219</v>
       </c>
@@ -2714,7 +2765,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>219</v>
       </c>
@@ -2734,7 +2785,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>219</v>
       </c>
@@ -2754,7 +2805,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>219</v>
       </c>
@@ -2774,7 +2825,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>219</v>
       </c>
@@ -2794,7 +2845,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>219</v>
       </c>
@@ -2814,7 +2865,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>219</v>
       </c>
@@ -2834,7 +2885,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>219</v>
       </c>
@@ -2854,7 +2905,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>219</v>
       </c>
@@ -2874,7 +2925,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>219</v>
       </c>
@@ -2894,7 +2945,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>219</v>
       </c>
@@ -2914,7 +2965,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>219</v>
       </c>
@@ -2934,7 +2985,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>219</v>
       </c>
@@ -2954,7 +3005,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>219</v>
       </c>
@@ -2974,7 +3025,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>219</v>
       </c>
@@ -2994,7 +3045,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>219</v>
       </c>
@@ -3014,7 +3065,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>219</v>
       </c>
@@ -3034,7 +3085,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>219</v>
       </c>
@@ -3054,7 +3105,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>219</v>
       </c>
@@ -3074,7 +3125,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>219</v>
       </c>
@@ -3094,7 +3145,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>219</v>
       </c>
@@ -3114,7 +3165,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>219</v>
       </c>
@@ -3134,7 +3185,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>219</v>
       </c>
@@ -3154,7 +3205,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>219</v>
       </c>
@@ -3174,7 +3225,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>219</v>
       </c>
@@ -3194,7 +3245,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>219</v>
       </c>
@@ -3214,7 +3265,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>219</v>
       </c>
@@ -3234,7 +3285,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>219</v>
       </c>
@@ -3254,7 +3305,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>219</v>
       </c>
@@ -3274,7 +3325,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>219</v>
       </c>
@@ -3294,7 +3345,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>219</v>
       </c>
@@ -3314,7 +3365,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>219</v>
       </c>
@@ -3334,7 +3385,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>219</v>
       </c>
@@ -3354,7 +3405,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>252</v>
       </c>
@@ -3368,7 +3419,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>219</v>
       </c>
@@ -3385,7 +3436,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>219</v>
       </c>
@@ -3402,7 +3453,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>258</v>
       </c>
@@ -3416,7 +3467,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>425</v>
       </c>
@@ -3430,7 +3481,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>260</v>
       </c>
@@ -3444,7 +3495,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>333</v>
       </c>
@@ -3458,7 +3509,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>219</v>
       </c>
@@ -3475,7 +3526,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>304</v>
       </c>
@@ -3489,7 +3540,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>219</v>
       </c>
@@ -3506,7 +3557,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>219</v>
       </c>
@@ -3523,7 +3574,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>219</v>
       </c>
@@ -3540,7 +3591,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>313</v>
       </c>
@@ -3554,7 +3605,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>219</v>
       </c>
@@ -3571,7 +3622,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>219</v>
       </c>
@@ -3588,7 +3639,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>219</v>
       </c>
@@ -3605,7 +3656,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>219</v>
       </c>
@@ -3622,7 +3673,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>365</v>
       </c>
@@ -3636,7 +3687,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>219</v>
       </c>
@@ -3653,7 +3704,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>219</v>
       </c>
@@ -3670,7 +3721,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>219</v>
       </c>
@@ -3687,7 +3738,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>359</v>
       </c>
@@ -3701,7 +3752,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>385</v>
       </c>
@@ -3718,7 +3769,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>219</v>
       </c>
@@ -3735,7 +3786,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>219</v>
       </c>
@@ -3752,7 +3803,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>335</v>
       </c>
@@ -3766,7 +3817,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>337</v>
       </c>
@@ -3780,7 +3831,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>219</v>
       </c>
@@ -3797,7 +3848,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>219</v>
       </c>
@@ -3814,7 +3865,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>219</v>
       </c>
@@ -3831,7 +3882,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>219</v>
       </c>
@@ -3848,7 +3899,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>343</v>
       </c>
@@ -3862,7 +3913,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>219</v>
       </c>
@@ -3879,7 +3930,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>302</v>
       </c>
@@ -3893,7 +3944,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>345</v>
       </c>
@@ -3907,7 +3958,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>367</v>
       </c>
@@ -3921,7 +3972,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>219</v>
       </c>
@@ -3938,7 +3989,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>219</v>
       </c>
@@ -3955,7 +4006,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>219</v>
       </c>
@@ -3972,7 +4023,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>219</v>
       </c>
@@ -3989,7 +4040,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>219</v>
       </c>
@@ -4006,7 +4057,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>219</v>
       </c>
@@ -4023,7 +4074,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>363</v>
       </c>
@@ -4037,7 +4088,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>219</v>
       </c>
@@ -4054,7 +4105,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>219</v>
       </c>
@@ -4071,7 +4122,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>219</v>
       </c>
@@ -4088,7 +4139,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>219</v>
       </c>
@@ -4105,7 +4156,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>220</v>
       </c>
@@ -4119,7 +4170,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>277</v>
       </c>
@@ -4133,7 +4184,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>219</v>
       </c>
@@ -4150,7 +4201,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>281</v>
       </c>
@@ -4164,7 +4215,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>219</v>
       </c>
@@ -4181,7 +4232,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>219</v>
       </c>
@@ -4198,7 +4249,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>219</v>
       </c>
@@ -4215,7 +4266,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>380</v>
       </c>
@@ -4229,7 +4280,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>219</v>
       </c>
@@ -4246,7 +4297,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>225</v>
       </c>
@@ -4260,7 +4311,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>219</v>
       </c>
@@ -4277,7 +4328,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>219</v>
       </c>
@@ -4294,7 +4345,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>219</v>
       </c>
@@ -4311,7 +4362,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>219</v>
       </c>
@@ -4328,7 +4379,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>219</v>
       </c>
@@ -4345,7 +4396,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>219</v>
       </c>
@@ -4362,7 +4413,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>219</v>
       </c>
@@ -4379,7 +4430,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>219</v>
       </c>
@@ -4396,7 +4447,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>219</v>
       </c>
@@ -4413,7 +4464,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>219</v>
       </c>
@@ -4430,7 +4481,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>219</v>
       </c>
@@ -4447,7 +4498,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>219</v>
       </c>
@@ -4464,7 +4515,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>327</v>
       </c>
@@ -4478,7 +4529,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>219</v>
       </c>
@@ -4495,7 +4546,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>308</v>
       </c>
@@ -4509,7 +4560,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>219</v>
       </c>
@@ -4523,7 +4574,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>219</v>
       </c>
@@ -4537,7 +4588,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>386</v>
       </c>
@@ -4548,7 +4599,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>231</v>
       </c>
@@ -4559,7 +4610,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>387</v>
       </c>
@@ -4570,7 +4621,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>426</v>
       </c>
@@ -4581,7 +4632,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>388</v>
       </c>
@@ -4592,7 +4643,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>389</v>
       </c>
@@ -4603,7 +4654,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>219</v>
       </c>
@@ -4617,7 +4668,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>219</v>
       </c>
@@ -4631,7 +4682,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>244</v>
       </c>
@@ -4642,7 +4693,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>245</v>
       </c>
@@ -4653,7 +4704,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>390</v>
       </c>
@@ -4664,7 +4715,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>219</v>
       </c>
@@ -4678,7 +4729,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>219</v>
       </c>
@@ -4693,9 +4744,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D84:D170" xr:uid="{B675B9CC-E73B-0348-8E12-10D80F222CA5}">
+      <formula1>impact</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C111" r:id="rId1"/>
-    <hyperlink ref="C90" r:id="rId2"/>
+    <hyperlink ref="C111" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C90" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -4704,4 +4760,64 @@
   </headerFooter>
   <legacyDrawingHF r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E872A15-FB8C-4949-B148-EB6DD99CB009}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.1640625" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>